<commit_message>
update geo  and par_file to new specfem format
</commit_message>
<xml_diff>
--- a/DiggerDAS/DOC/logsheet.xlsx
+++ b/DiggerDAS/DOC/logsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rlnd\projects\DiggerDAS\DOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rlnd\gitclones\specfem-examples\DiggerDAS\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F18A1B-2800-480E-A80B-F89532056070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A961CB-BFC0-4423-957E-49F8DF3A2663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Logsheet DiggerDAS simulations</t>
   </si>
@@ -146,25 +146,79 @@
     <t>Hz</t>
   </si>
   <si>
-    <t>M1-air</t>
-  </si>
-  <si>
-    <t>M2-clay</t>
-  </si>
-  <si>
-    <t>M3_water</t>
-  </si>
-  <si>
-    <t>rho (kg/m3</t>
-  </si>
-  <si>
-    <t>vp (m/s)</t>
-  </si>
-  <si>
-    <t>vs (m/s)</t>
-  </si>
-  <si>
     <t>nbmodels</t>
+  </si>
+  <si>
+    <t>dens</t>
+  </si>
+  <si>
+    <t>vp</t>
+  </si>
+  <si>
+    <t>vs</t>
+  </si>
+  <si>
+    <t>qkappa</t>
+  </si>
+  <si>
+    <t>qmu</t>
+  </si>
+  <si>
+    <t># comment</t>
+  </si>
+  <si>
+    <t>1784.d0</t>
+  </si>
+  <si>
+    <t>1600.d0</t>
+  </si>
+  <si>
+    <t># clay with specific weight 17.5 kN/m3</t>
+  </si>
+  <si>
+    <t># sand with specific weight 18.5 kN/m3</t>
+  </si>
+  <si>
+    <t># water burrow entrance</t>
+  </si>
+  <si>
+    <t># air in burrow</t>
+  </si>
+  <si>
+    <t>1886.d0</t>
+  </si>
+  <si>
+    <t>1000.d0</t>
+  </si>
+  <si>
+    <t>1480.d0</t>
+  </si>
+  <si>
+    <t>0.000d0</t>
+  </si>
+  <si>
+    <t>1.000d0</t>
+  </si>
+  <si>
+    <t>343.0d0</t>
+  </si>
+  <si>
+    <t>500.0d0</t>
+  </si>
+  <si>
+    <t>400.0d0</t>
+  </si>
+  <si>
+    <t>1700.d0</t>
+  </si>
+  <si>
+    <t>ani</t>
+  </si>
+  <si>
+    <t>material_id</t>
+  </si>
+  <si>
+    <t>domain_id</t>
   </si>
 </sst>
 </file>
@@ -218,10 +272,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -505,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,6 +569,8 @@
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="34.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -524,10 +579,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -535,7 +590,7 @@
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -605,7 +660,7 @@
       <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>0.05</v>
       </c>
       <c r="K10" t="s">
@@ -638,12 +693,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="H17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -658,7 +713,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -671,7 +726,7 @@
       <c r="H19" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19">
         <f>1/C8/C19/2</f>
         <v>4999.9999999999991</v>
       </c>
@@ -679,7 +734,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -688,7 +743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -696,7 +751,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -704,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -712,82 +767,193 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H24" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C27">
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,H31:P31)</f>
+        <v>2 1 1784.d0 1700.d0 500.0d0 9999 9999 0 # clay with specific weight 17.5 kN/m3</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>43</v>
+      </c>
+      <c r="K31" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31" t="s">
+        <v>55</v>
+      </c>
+      <c r="M31">
+        <v>9999</v>
+      </c>
+      <c r="N31">
+        <v>9999</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,H32:P32)</f>
+        <v>2 2 1886.d0 1600.d0 400.0d0 9999 9999 0 # sand with specific weight 18.5 kN/m3</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>49</v>
+      </c>
+      <c r="K32" t="s">
+        <v>44</v>
+      </c>
+      <c r="L32" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32">
+        <v>9999</v>
+      </c>
+      <c r="N32">
+        <v>9999</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,H33:P33)</f>
+        <v>1 3 1000.d0 1480.d0 0.000d0 9999 9999 0 # water burrow entrance</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>50</v>
+      </c>
+      <c r="K33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L33" t="s">
+        <v>52</v>
+      </c>
+      <c r="M33">
+        <v>9999</v>
+      </c>
+      <c r="N33">
+        <v>9999</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,H34:P34)</f>
+        <v>1 4 1.000d0 343.0d0 0.000d0 9999 9999 0 # air in burrow</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
         <v>4</v>
       </c>
-      <c r="I27" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" t="s">
-        <v>40</v>
-      </c>
-      <c r="K27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H28" t="s">
-        <v>36</v>
-      </c>
-      <c r="I28">
-        <v>1.2929999999999999</v>
-      </c>
-      <c r="J28">
-        <v>343</v>
-      </c>
-      <c r="K28">
+      <c r="J34" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" t="s">
+        <v>54</v>
+      </c>
+      <c r="L34" t="s">
+        <v>52</v>
+      </c>
+      <c r="M34">
+        <v>9999</v>
+      </c>
+      <c r="N34">
+        <v>9999</v>
+      </c>
+      <c r="O34">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H29" t="s">
-        <v>37</v>
-      </c>
-      <c r="I29">
-        <v>1600</v>
-      </c>
-      <c r="J29">
-        <v>1600</v>
-      </c>
-      <c r="K29">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H30" t="s">
-        <v>38</v>
-      </c>
-      <c r="I30">
-        <v>1000</v>
-      </c>
-      <c r="J30">
-        <v>1480</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
+      <c r="P34" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cfl pp lambda conditons in readme
</commit_message>
<xml_diff>
--- a/DiggerDAS/DOC/logsheet.xlsx
+++ b/DiggerDAS/DOC/logsheet.xlsx
@@ -8,12 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rlnd\gitclones\specfem-examples\DiggerDAS\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A961CB-BFC0-4423-957E-49F8DF3A2663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686E9B79-869B-4BB9-B859-AD5FA1DA78B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12675" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Logsheet model runs" sheetId="6" r:id="rId1"/>
+    <sheet name="Par_file" sheetId="1" r:id="rId2"/>
+    <sheet name="SOURCE" sheetId="2" r:id="rId3"/>
+    <sheet name="schema.geo" sheetId="3" r:id="rId4"/>
+    <sheet name="nummaterial_velocity_file" sheetId="4" r:id="rId5"/>
+    <sheet name="Questions" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="101">
   <si>
     <t>Logsheet DiggerDAS simulations</t>
   </si>
@@ -92,18 +97,6 @@
     <t>zfin</t>
   </si>
   <si>
-    <t>In SOURCE file</t>
-  </si>
-  <si>
-    <t>xs</t>
-  </si>
-  <si>
-    <t>zs</t>
-  </si>
-  <si>
-    <t>BCs</t>
-  </si>
-  <si>
     <t>PML</t>
   </si>
   <si>
@@ -149,9 +142,6 @@
     <t>nbmodels</t>
   </si>
   <si>
-    <t>dens</t>
-  </si>
-  <si>
     <t>vp</t>
   </si>
   <si>
@@ -219,6 +209,141 @@
   </si>
   <si>
     <t>domain_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             </t>
+  </si>
+  <si>
+    <t>spaces</t>
+  </si>
+  <si>
+    <t>#(1)domain_id #(2)material_id #(3)rho #(4)vp #(5)vs #(6)Q_k #(7)Q_mu #(8)ani</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>lc</t>
+  </si>
+  <si>
+    <t>free surface</t>
+  </si>
+  <si>
+    <t>lc/2</t>
+  </si>
+  <si>
+    <t>around hole</t>
+  </si>
+  <si>
+    <t>lc/4</t>
+  </si>
+  <si>
+    <t>directions are vital</t>
+  </si>
+  <si>
+    <t>all line loops should be defined countclockwise (you might have to set line sections to negative to make this work</t>
+  </si>
+  <si>
+    <t>neg_material_id</t>
+  </si>
+  <si>
+    <t>tomo file name</t>
+  </si>
+  <si>
+    <t>tomo.xyz</t>
+  </si>
+  <si>
+    <t>pos_unique_id</t>
+  </si>
+  <si>
+    <t>tomography elastic</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t># tomography through clay</t>
+  </si>
+  <si>
+    <t>schema0</t>
+  </si>
+  <si>
+    <t>clay layer over sandlayer</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>same but invluding a beaver hole with entrence from below filled with water and 'chamber' filled with air</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Par_file</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>source_type</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>Standard elastic fors/acoustic pressure, or use intial field type with p-wave, s-wave or rayleigh wave (consider interferometry on river dike</t>
+  </si>
+  <si>
+    <t>mesh</t>
+  </si>
+  <si>
+    <t>schema1</t>
+  </si>
+  <si>
+    <t>source type</t>
+  </si>
+  <si>
+    <t>elastic force</t>
+  </si>
+  <si>
+    <t>schema2</t>
+  </si>
+  <si>
+    <t>schema3</t>
+  </si>
+  <si>
+    <t>schema4</t>
+  </si>
+  <si>
+    <t>schema5</t>
+  </si>
+  <si>
+    <t>schema6</t>
+  </si>
+  <si>
+    <t>schema7</t>
+  </si>
+  <si>
+    <t>schema8</t>
+  </si>
+  <si>
+    <t>schema9</t>
+  </si>
+  <si>
+    <t>initial field</t>
+  </si>
+  <si>
+    <t>ps</t>
+  </si>
+  <si>
+    <t>rayleigh</t>
   </si>
 </sst>
 </file>
@@ -228,7 +353,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,16 +376,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -268,16 +420,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,11 +768,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{334FB5FD-5CEE-4D11-A398-A4F3457A8FCE}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,177 +907,162 @@
     <col min="8" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>0.5</v>
-      </c>
-      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>10</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>2</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>300</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <f>J10/C8</f>
-        <v>5000</v>
-      </c>
-      <c r="H9" t="s">
+        <f>K10/C8</f>
+        <v>500000.00000000006</v>
+      </c>
+      <c r="I9" t="s">
         <v>4</v>
       </c>
-      <c r="J9">
-        <f>J7/J8</f>
+      <c r="K9">
+        <f>K7/K8</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>0.05</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H11" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
         <v>11</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H12" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
         <v>12</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H17" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1">
         <f>2*C9</f>
-        <v>10000</v>
+        <v>1000000.0000000001</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I19">
-        <f>1/C8/C19/2</f>
-        <v>4999.9999999999991</v>
-      </c>
-      <c r="J19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="I19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19">
+        <v>30</v>
+      </c>
+      <c r="K19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="C20">
-        <f>(J7-1)/0.5+1</f>
+        <f>(K7-1)/0.5+1</f>
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -751,7 +1070,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -759,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -767,193 +1086,447 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="H30" s="3" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F958B4C-6881-487A-9A08-DA44691D7CD6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E751F6D2-B667-4BC3-840B-0C673216120E}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="B1">
+        <v>0.2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BDE741-63B3-405A-99ED-1290335B1FDE}">
+  <dimension ref="A1:L10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.21875" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="92.109375" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" customWidth="1"/>
+    <col min="18" max="18" width="8.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="L1" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="D2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="6">
+        <v>9999</v>
+      </c>
+      <c r="G2" s="6">
+        <v>9999</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="8" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A2:J2)</f>
+        <v>2 1 1784.d0 1700.d0 500.0d0 9999 9999 0               # clay with specific weight 17.5 kN/m3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M30" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N30" s="3" t="s">
+      <c r="E3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="6">
+        <v>9999</v>
+      </c>
+      <c r="G3" s="6">
+        <v>9999</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P30" s="3" t="s">
+      <c r="L3" s="8" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A3:J3)</f>
+        <v>2 2 1886.d0 1600.d0 400.0d0 9999 9999 0               # sand with specific weight 18.5 kN/m3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="6">
+        <v>9999</v>
+      </c>
+      <c r="G4" s="6">
+        <v>9999</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,H31:P31)</f>
-        <v>2 1 1784.d0 1700.d0 500.0d0 9999 9999 0 # clay with specific weight 17.5 kN/m3</v>
-      </c>
-      <c r="H31">
+      <c r="L4" s="8" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A4:J4)</f>
+        <v>1 3 1000.d0 1480.d0 0.000d0 9999 9999 0               # water burrow entrance</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="6">
+        <v>9999</v>
+      </c>
+      <c r="G5" s="6">
+        <v>9999</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="9" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A5:J5)</f>
+        <v>1 4 1.000d0 343.0d0 0.000d0 9999 9999 0               # air in burrow</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L6" s="10" t="str">
+        <f t="shared" ref="L6:L10" si="0">_xlfn.TEXTJOIN(" ",TRUE,A6:J6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="L9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>domain_id neg_material_id description tomo file name pos_unique_id</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
         <v>2</v>
       </c>
-      <c r="I31">
+      <c r="B10" s="6">
+        <v>-1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="6">
         <v>1</v>
       </c>
-      <c r="J31" t="s">
-        <v>43</v>
-      </c>
-      <c r="K31" t="s">
-        <v>57</v>
-      </c>
-      <c r="L31" t="s">
-        <v>55</v>
-      </c>
-      <c r="M31">
-        <v>9999</v>
-      </c>
-      <c r="N31">
-        <v>9999</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,H32:P32)</f>
-        <v>2 2 1886.d0 1600.d0 400.0d0 9999 9999 0 # sand with specific weight 18.5 kN/m3</v>
-      </c>
-      <c r="H32">
-        <v>2</v>
-      </c>
-      <c r="I32">
-        <v>2</v>
-      </c>
-      <c r="J32" t="s">
-        <v>49</v>
-      </c>
-      <c r="K32" t="s">
-        <v>44</v>
-      </c>
-      <c r="L32" t="s">
-        <v>56</v>
-      </c>
-      <c r="M32">
-        <v>9999</v>
-      </c>
-      <c r="N32">
-        <v>9999</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,H33:P33)</f>
-        <v>1 3 1000.d0 1480.d0 0.000d0 9999 9999 0 # water burrow entrance</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>3</v>
-      </c>
-      <c r="J33" t="s">
-        <v>50</v>
-      </c>
-      <c r="K33" t="s">
-        <v>51</v>
-      </c>
-      <c r="L33" t="s">
-        <v>52</v>
-      </c>
-      <c r="M33">
-        <v>9999</v>
-      </c>
-      <c r="N33">
-        <v>9999</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,H34:P34)</f>
-        <v>1 4 1.000d0 343.0d0 0.000d0 9999 9999 0 # air in burrow</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <v>4</v>
-      </c>
-      <c r="J34" t="s">
-        <v>53</v>
-      </c>
-      <c r="K34" t="s">
-        <v>54</v>
-      </c>
-      <c r="L34" t="s">
-        <v>52</v>
-      </c>
-      <c r="M34">
-        <v>9999</v>
-      </c>
-      <c r="N34">
-        <v>9999</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34" t="s">
-        <v>48</v>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>2 -1 tomography elastic tomo.xyz 1 # tomography through clay</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EA09D4-74AA-41B0-9C9B-64DCA077C07B}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="31" style="11" customWidth="1"/>
+    <col min="4" max="4" width="197.44140625" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="11">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>